<commit_message>
added site/ to gitignore
</commit_message>
<xml_diff>
--- a/docs/jupyter_notebooks/tweet_dataset.xlsx
+++ b/docs/jupyter_notebooks/tweet_dataset.xlsx
@@ -37,6 +37,9 @@
     <t>Hashtags</t>
   </si>
   <si>
+    <t>Using #paytience on #tsla pays off when you are on the mic.   I would have never thought i'd make more day trading than working!  #x5 is coming soon enough, time to start scaling!     @tradewithMAK and @tradewithmak2 are printing money! 🏌️‍♂️🏌️‍♂️ https://t.co/RmNv9brKzq</t>
+  </si>
+  <si>
     <t>⁦@POTUS⁩ ⁦@VP⁩ ⁦@SenSanders⁩ ⁦@SenWarren⁩ ⁦so this is how good jobs are created?  That is inly if your employer is more ammoral than the ⁦@UAW⁩.  $TSLA #TSLA ⁦@elonmusk⁩ IS BETTER THAN THE UNIONS🚀🚀🚀 https://t.co/46WHJOUYoz</t>
   </si>
   <si>
@@ -208,20 +211,12 @@
     <t>What does the last sentence mean about isolation is difficult to move stock.  Are they saying 1100 is where it should be now according to them ?  $tsla #TSLA https://t.co/HBvp39zjNc</t>
   </si>
   <si>
-    <t>$TSLA Huge 🚀🚀🚀will cross $1600 this week. Why? Love it !!!
-🚀GigaTexas. 
-🚀15K guests invited.
-🚀Massive Call volume &amp;gt; 1200.
-🚀Stock SPLIT happening! CONFIRMED BY #TSLA. 
-Also lets buy these hot picks👇100%ers
-$PME 🚀
-$MRKR 🚀
-$THM</t>
-  </si>
-  <si>
     <t>2022-03-29</t>
   </si>
   <si>
+    <t>2022-01-26</t>
+  </si>
+  <si>
     <t>2021-12-18</t>
   </si>
   <si>
@@ -342,7 +337,7 @@
     <t>2018-11-04</t>
   </si>
   <si>
-    <t>2021-10-18</t>
+    <t>[{'text': 'paytience', 'indices': [6, 16]}, {'text': 'tsla', 'indices': [20, 25]}, {'text': 'x5', 'indices': [130, 133]}]</t>
   </si>
   <si>
     <t>[{'text': 'TSLA', 'indices': [152, 157]}]</t>
@@ -481,9 +476,6 @@
   </si>
   <si>
     <t>[{'text': 'TSLA', 'indices': [17, 22]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [163, 168]}]</t>
   </si>
 </sst>
 </file>
@@ -878,7 +870,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -904,7 +896,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>57</v>
@@ -930,7 +922,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
@@ -956,7 +948,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>57</v>
@@ -982,7 +974,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
@@ -1008,7 +1000,7 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>
@@ -1034,7 +1026,7 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>331</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
         <v>57</v>
@@ -1060,13 +1052,13 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>2309</v>
+        <v>331</v>
       </c>
       <c r="D9" t="s">
         <v>57</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1086,13 +1078,13 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>97</v>
+        <v>2309</v>
       </c>
       <c r="D10" t="s">
         <v>57</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1112,13 +1104,13 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
         <v>57</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1138,7 +1130,7 @@
         <v>17</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
         <v>57</v>
@@ -1176,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
         <v>110</v>
@@ -1190,7 +1182,7 @@
         <v>19</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>57</v>
@@ -1216,7 +1208,7 @@
         <v>20</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
         <v>57</v>
@@ -1228,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H15" t="s">
         <v>112</v>
@@ -1242,7 +1234,7 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>3136</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
@@ -1254,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H16" t="s">
         <v>113</v>
@@ -1268,7 +1260,7 @@
         <v>22</v>
       </c>
       <c r="C17">
-        <v>40</v>
+        <v>3136</v>
       </c>
       <c r="D17" t="s">
         <v>57</v>
@@ -1294,7 +1286,7 @@
         <v>23</v>
       </c>
       <c r="C18">
-        <v>823</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>57</v>
@@ -1320,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>823</v>
       </c>
       <c r="D19" t="s">
         <v>57</v>
@@ -1358,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
         <v>117</v>
@@ -1372,7 +1364,7 @@
         <v>26</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
@@ -1398,7 +1390,7 @@
         <v>27</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
         <v>57</v>
@@ -1424,7 +1416,7 @@
         <v>28</v>
       </c>
       <c r="C23">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
         <v>57</v>
@@ -1450,7 +1442,7 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
         <v>57</v>
@@ -1462,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="H24" t="s">
         <v>121</v>
@@ -1476,7 +1468,7 @@
         <v>30</v>
       </c>
       <c r="C25">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
         <v>57</v>
@@ -1488,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
         <v>122</v>
@@ -1502,7 +1494,7 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
         <v>57</v>
@@ -1528,7 +1520,7 @@
         <v>32</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>57</v>
@@ -1554,7 +1546,7 @@
         <v>33</v>
       </c>
       <c r="C28">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
         <v>57</v>
@@ -1566,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="H28" t="s">
         <v>125</v>
@@ -1580,7 +1572,7 @@
         <v>34</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
         <v>57</v>
@@ -1592,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
@@ -1606,13 +1598,13 @@
         <v>35</v>
       </c>
       <c r="C30">
-        <v>1146</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
         <v>57</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -1632,13 +1624,13 @@
         <v>36</v>
       </c>
       <c r="C31">
-        <v>949</v>
+        <v>1147</v>
       </c>
       <c r="D31" t="s">
         <v>57</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -1658,7 +1650,7 @@
         <v>37</v>
       </c>
       <c r="C32">
-        <v>226</v>
+        <v>949</v>
       </c>
       <c r="D32" t="s">
         <v>57</v>
@@ -1684,7 +1676,7 @@
         <v>38</v>
       </c>
       <c r="C33">
-        <v>797</v>
+        <v>226</v>
       </c>
       <c r="D33" t="s">
         <v>57</v>
@@ -1710,7 +1702,7 @@
         <v>39</v>
       </c>
       <c r="C34">
-        <v>629</v>
+        <v>797</v>
       </c>
       <c r="D34" t="s">
         <v>57</v>
@@ -1736,7 +1728,7 @@
         <v>40</v>
       </c>
       <c r="C35">
-        <v>460</v>
+        <v>629</v>
       </c>
       <c r="D35" t="s">
         <v>57</v>
@@ -1762,7 +1754,7 @@
         <v>41</v>
       </c>
       <c r="C36">
-        <v>127</v>
+        <v>460</v>
       </c>
       <c r="D36" t="s">
         <v>57</v>
@@ -1788,7 +1780,7 @@
         <v>42</v>
       </c>
       <c r="C37">
-        <v>94</v>
+        <v>127</v>
       </c>
       <c r="D37" t="s">
         <v>57</v>
@@ -1826,10 +1818,10 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1852,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H39" t="s">
         <v>135</v>
@@ -1878,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H40" t="s">
         <v>136</v>
@@ -1904,7 +1896,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H41" t="s">
         <v>137</v>
@@ -1918,7 +1910,7 @@
         <v>47</v>
       </c>
       <c r="C42">
-        <v>269</v>
+        <v>94</v>
       </c>
       <c r="D42" t="s">
         <v>57</v>
@@ -1944,7 +1936,7 @@
         <v>48</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>269</v>
       </c>
       <c r="D43" t="s">
         <v>57</v>
@@ -1970,7 +1962,7 @@
         <v>49</v>
       </c>
       <c r="C44">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
         <v>57</v>
@@ -1996,7 +1988,7 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>1341</v>
+        <v>53</v>
       </c>
       <c r="D45" t="s">
         <v>57</v>
@@ -2022,7 +2014,7 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>10</v>
+        <v>1341</v>
       </c>
       <c r="D46" t="s">
         <v>57</v>
@@ -2048,7 +2040,7 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>3257</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
         <v>57</v>
@@ -2074,7 +2066,7 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>781</v>
+        <v>3257</v>
       </c>
       <c r="D48" t="s">
         <v>57</v>
@@ -2100,7 +2092,7 @@
         <v>54</v>
       </c>
       <c r="C49">
-        <v>118</v>
+        <v>781</v>
       </c>
       <c r="D49" t="s">
         <v>57</v>
@@ -2115,7 +2107,7 @@
         <v>96</v>
       </c>
       <c r="H49" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2126,7 +2118,7 @@
         <v>55</v>
       </c>
       <c r="C50">
-        <v>266</v>
+        <v>118</v>
       </c>
       <c r="D50" t="s">
         <v>57</v>
@@ -2141,7 +2133,7 @@
         <v>97</v>
       </c>
       <c r="H50" t="s">
-        <v>99</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2152,7 +2144,7 @@
         <v>56</v>
       </c>
       <c r="C51">
-        <v>23</v>
+        <v>266</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
@@ -2167,7 +2159,7 @@
         <v>98</v>
       </c>
       <c r="H51" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#docs wrote Social Media Docs and Twint Test
</commit_message>
<xml_diff>
--- a/docs/jupyter_notebooks/tweet_dataset.xlsx
+++ b/docs/jupyter_notebooks/tweet_dataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="180">
   <si>
     <t>Tweet</t>
   </si>
@@ -37,452 +37,586 @@
     <t>Hashtags</t>
   </si>
   <si>
-    <t>Using #paytience on #tsla pays off when you are on the mic.   I would have never thought i'd make more day trading than working!  #x5 is coming soon enough, time to start scaling!     @tradewithMAK and @tradewithmak2 are printing money! 🏌️‍♂️🏌️‍♂️ https://t.co/RmNv9brKzq</t>
-  </si>
-  <si>
-    <t>⁦@POTUS⁩ ⁦@VP⁩ ⁦@SenSanders⁩ ⁦@SenWarren⁩ ⁦so this is how good jobs are created?  That is inly if your employer is more ammoral than the ⁦@UAW⁩.  $TSLA #TSLA ⁦@elonmusk⁩ IS BETTER THAN THE UNIONS🚀🚀🚀 https://t.co/46WHJOUYoz</t>
-  </si>
-  <si>
-    <t>Gym ✅
-$1,171.25 from the market today✅
-#LetsRide #gym #stocks #TSLA</t>
-  </si>
-  <si>
-    <t>love Sara Eisen quote today on #cnbc, #TSLA is up 8% this week and it’s only Tuesday. Love it!</t>
-  </si>
-  <si>
-    <t>Not everyday you get 10% in 3 mins on a big cap #amc #gme #tsla #hymc #hood #daytrading https://t.co/towJiMmaMy</t>
-  </si>
-  <si>
-    <t>@userofintellect @TOFIQFAZL Rather worrying to see #TSLA following #AMC movements today.</t>
-  </si>
-  <si>
-    <t>@elonmusk isn’t it crazy that the @SEC_Enforcement is wasting our taxpayer dollars harassing you, when there’s firms like @citidelsec that blatantly manipulate our markets and steal from the very taxpayers that fund the SEC?! This shit is a joke #TSLA #AMC #GME  #ShortSqueeze</t>
-  </si>
-  <si>
-    <t>Open: $1,107.99
-Close: $1,099.57
-Range: $1,073.11 - $1,114.76
-It’s not too late to buy #TSLA</t>
-  </si>
-  <si>
-    <t>“the federal government has announced some $9.1 billion in new investments that will, among other things, boost incentives for zero-emission vehicles”
-#CanadaNickel 
-#SudburyTwoPointO
-#NetZeroNickel 
-#Nickel  $CNIKF
-$CNC.V  #EV  #TSLA #ESG # 
-#Glencore #BHP #Vale #Canada https://t.co/WFZrLIXP3L</t>
-  </si>
-  <si>
-    <t>@SawyerMerritt @elonmusk Funny Teamsters 9y ago stole 20million from the union I was a part of, they had to settle out of court(2019) and workers all received settlements which I 100% put it all in #TSLA 🤑, the investment made me +10x and counting, I guess some good cane out of this debacle, hate unions</t>
-  </si>
-  <si>
-    <t>How the fuck is the $vix at 18 rn?! #tsla $tsla</t>
-  </si>
-  <si>
-    <t>@davidgarcialou Do you think #TSLA can go up to 1200 in the near future?</t>
-  </si>
-  <si>
-    <t>@browncs555 Do you think #TSLA can go up to 1200 in the near future?</t>
-  </si>
-  <si>
-    <t>#TSLA WILL DO 5-1 Solit</t>
-  </si>
-  <si>
-    <t>@JohnDur68716211 Do you think #TSLA can go up to 1200 in the near future?</t>
-  </si>
-  <si>
-    <t>$TSLA one of the most mentioned on wallstreetbets over the last 24 hours_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #stocks https://t.co/3ghWO3Fvy8</t>
-  </si>
-  <si>
-    <t>Why don't Apple &amp;amp; Telsa split their stock every week. The we can get the SPX to 10,000 in no time at all.😂 #AAPL $AAPL $TSLA #TSLA $SPX #NDX</t>
-  </si>
-  <si>
-    <t>I’m not sure how it is in other, larger Canadian cities, but I feel like Winnipeg is going to be a pain in Teslas ass for training FSD - our streets are absolutely terrible #TSLA #FSDBetaCanada</t>
-  </si>
-  <si>
-    <t>#TSLA #Tesla #Elon #ElonMusk Utttt oh.
-PS #Bitcoin #BTC follows Tesla. Look for yourself. https://t.co/dYFRePI7Di</t>
-  </si>
-  <si>
-    <t>Shorting #TSLA #Tesla #Elon #ElonMusk with my life! https://t.co/cdXYiNN2Pr</t>
-  </si>
-  <si>
-    <t>How it started VS how it’s going #tesla #builtTentTough #tsla @moonchic #musked when a company fucks you, best to tweet at them and worlds richest person and start tweet with I love my tesla but #rookiemistake https://t.co/sfo4p8kxH8</t>
-  </si>
-  <si>
-    <t>@elonmusk @SawyerMerritt Would #TSLA ever go union?</t>
-  </si>
-  <si>
-    <t>This seems ...important #ev #tsla #GreenNewDeal https://t.co/LUpRZRHH5u</t>
-  </si>
-  <si>
-    <t>@R_macroe Parabolic move coming...we are breaking through all time highs soon $LCID #ev #ElectricVehicles #TSLA</t>
-  </si>
-  <si>
-    <t>@TeslaBest @Tesla @elonmusk #TSLA $1,103 right now !</t>
-  </si>
-  <si>
-    <t>@elonmusk We all know EV is the future. Please consider adding more charging stations at AMC parking lots. Plenty of space at the back lots as everyone fights to get the closes parking during movie nights. Thank you.  #TSLA #AMC $TSLA $AMC</t>
-  </si>
-  <si>
-    <t>Bears are finally going to get their $300 $TSLA stock price soon. 
-But it’ll be the result of a 4:1 split.😂😂
-#TSLA #StockMarket</t>
-  </si>
-  <si>
-    <t>At what point does Tesla miss expectations and the stock crashes 25% in a day? #TSLA $TSLA</t>
-  </si>
-  <si>
-    <t>Largest stock positions are: #PLTR, #NIO, #TSLA, and #RIOT 🚀</t>
-  </si>
-  <si>
-    <t>(3/14)
-ie buying #HBAR with #TSLA shares! A bot that will trade for you, paying for coffee with your Hbar, and very exciting too; vaults! (read on)
-This infographic shows where they are positioning themselves. https://t.co/01gqozGYhY</t>
-  </si>
-  <si>
-    <t>𝗦𝘁𝗼𝗰𝗸𝘀 𝗛𝗶𝘁 𝗦𝗶𝘅-𝗪𝗲𝗲𝗸 𝗛𝗶𝗴𝗵!
-#Tesla (#TSLA) CEO Elon Musk announced that the firm will seek another stock split in the near future, triggering a near-double-digit surge in its shares..
-Read More: https://t.co/L2l1NrEjl5
-#StockBuzzNow #stockmarkettips #usamarket https://t.co/mXBsBXzTFH</t>
-  </si>
-  <si>
-    <t>Tesla do your thing and push another split of 1:10 #TSLA</t>
-  </si>
-  <si>
-    <t>LIMITED TIME OFFER: Get 5 FREE stocks valued up to $9,600 by opening &amp;amp; funding a #Webull brokerage account! Get started &amp;gt; #BTC    #MMAT #TSLA #YOMTVRaps #HipHop #Verzuz #NFT #Stocks #Stockmarket #NFTCommunity #CarlosEMendez https://t.co/YqRmgEv99k https://t.co/OgerHwuyRT</t>
-  </si>
-  <si>
-    <t>2021 is just the beginning for #EVs with 6.5M EVs sold worldwide. Automakers are racing to take it into its next phase. But who will be the biggest winner? Join Lynk Learning webinar (https://t.co/U55spR1Iwb) to know why the time for EVs is NOW!
-#TSLA #F #GM #LCID #RIVN #NIO https://t.co/liC6QUefv4</t>
-  </si>
-  <si>
-    <t>shorted $TSLA today ,should atleast go for that gap fill, which is already gonna be around 8%
-#TSLA #Tesla https://t.co/GTyRXoLj6D https://t.co/1KjX9UmplD</t>
-  </si>
-  <si>
-    <t>Day 5! Green Day keeps the doctor away. 6 days green in a row, feeling good 
-#options #daytrading #spy #tsla #amc https://t.co/tY7rqgTBwi</t>
-  </si>
-  <si>
-    <t>@NKozev The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@WK3499 The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@ThorbenGroth @WholeMarsBlog @SawyerMerritt The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@StockNewsOutlet The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>@MorgenMedien The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
-  </si>
-  <si>
-    <t>Tesla..What Can You Say!! #tesla #tsla #stock #stockmarket #options #money #cars #tech #technology https://t.co/WFQqkW6U40</t>
-  </si>
-  <si>
-    <t>@$TSLA #tsla I am an enthusiastic Tesla stockholder and soon to be owner. I will be in Austin for the incredible event. Hoping to score a +1 ticket @elonmusk $TSLA anyone?</t>
-  </si>
-  <si>
-    <t>Call me a radical #TSLA junkie cultist @WholeMarsBlog but I believe it’s the @NHTSAgov to protect civil-operators of a motor-vehicle &amp;amp; not drag names like @Tesla checks notes *with zero deaths* for having a hard time avoiding checks notes *maneuvering around safety-units?</t>
-  </si>
-  <si>
-    <t>@TeslaAndDoge No, IMO #TSLA will reach 
-$2022 before the end of 2022.🤡</t>
-  </si>
-  <si>
-    <t>Looks like #TSLA will be the first to break new ATH since this stock market correction.</t>
-  </si>
-  <si>
-    <t>@WSBArmy Remember to add #doge and #tsla
-👍</t>
-  </si>
-  <si>
-    <t>It’s nice to see #TSLA green once more! ♥️ https://t.co/YCHMcGmuht</t>
-  </si>
-  <si>
-    <t>Thoughts on $TSLA #TSLA! See drsyariz's idea on TradingView below. https://t.co/2ZzLLNunHF</t>
-  </si>
-  <si>
-    <t>What does the last sentence mean about isolation is difficult to move stock.  Are they saying 1100 is where it should be now according to them ?  $tsla #TSLA https://t.co/HBvp39zjNc</t>
-  </si>
-  <si>
-    <t>2022-03-29</t>
-  </si>
-  <si>
-    <t>2022-01-26</t>
-  </si>
-  <si>
-    <t>2021-12-18</t>
-  </si>
-  <si>
-    <t>2018-12-15</t>
-  </si>
-  <si>
-    <t>2021-11-10</t>
-  </si>
-  <si>
-    <t>2021-12-12</t>
-  </si>
-  <si>
-    <t>2020-04-30</t>
-  </si>
-  <si>
-    <t>2021-06-24</t>
-  </si>
-  <si>
-    <t>2021-10-28</t>
-  </si>
-  <si>
-    <t>2015-03-15</t>
-  </si>
-  <si>
-    <t>2020-07-20</t>
-  </si>
-  <si>
-    <t>2020-06-29</t>
-  </si>
-  <si>
-    <t>2022-03-28</t>
-  </si>
-  <si>
-    <t>2018-05-04</t>
-  </si>
-  <si>
-    <t>2020-01-08</t>
-  </si>
-  <si>
-    <t>2018-06-08</t>
-  </si>
-  <si>
-    <t>2019-11-03</t>
-  </si>
-  <si>
-    <t>2022-03-06</t>
-  </si>
-  <si>
-    <t>2021-11-14</t>
-  </si>
-  <si>
-    <t>2017-07-12</t>
-  </si>
-  <si>
-    <t>2020-07-06</t>
-  </si>
-  <si>
-    <t>2012-09-03</t>
-  </si>
-  <si>
-    <t>2021-12-14</t>
-  </si>
-  <si>
-    <t>2022-03-10</t>
-  </si>
-  <si>
-    <t>2021-04-27</t>
-  </si>
-  <si>
-    <t>2021-05-16</t>
-  </si>
-  <si>
-    <t>2009-06-12</t>
-  </si>
-  <si>
-    <t>2015-10-20</t>
-  </si>
-  <si>
-    <t>2013-01-29</t>
-  </si>
-  <si>
-    <t>2013-10-01</t>
-  </si>
-  <si>
-    <t>2015-08-23</t>
-  </si>
-  <si>
-    <t>2018-07-25</t>
-  </si>
-  <si>
-    <t>2010-12-06</t>
-  </si>
-  <si>
-    <t>2017-08-04</t>
-  </si>
-  <si>
-    <t>2018-04-10</t>
-  </si>
-  <si>
-    <t>2021-09-28</t>
-  </si>
-  <si>
-    <t>2009-07-30</t>
-  </si>
-  <si>
-    <t>2021-08-11</t>
-  </si>
-  <si>
-    <t>2021-05-10</t>
-  </si>
-  <si>
-    <t>2015-08-04</t>
-  </si>
-  <si>
-    <t>2020-09-29</t>
-  </si>
-  <si>
-    <t>2018-11-04</t>
-  </si>
-  <si>
-    <t>[{'text': 'paytience', 'indices': [6, 16]}, {'text': 'tsla', 'indices': [20, 25]}, {'text': 'x5', 'indices': [130, 133]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [152, 157]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'LetsRide', 'indices': [39, 48]}, {'text': 'gym', 'indices': [49, 53]}, {'text': 'stocks', 'indices': [54, 61]}, {'text': 'TSLA', 'indices': [62, 67]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'cnbc', 'indices': [31, 36]}, {'text': 'TSLA', 'indices': [38, 43]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'amc', 'indices': [48, 52]}, {'text': 'gme', 'indices': [53, 57]}, {'text': 'tsla', 'indices': [58, 63]}, {'text': 'hymc', 'indices': [64, 69]}, {'text': 'hood', 'indices': [70, 75]}, {'text': 'daytrading', 'indices': [76, 87]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [51, 56]}, {'text': 'AMC', 'indices': [67, 71]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [246, 251]}, {'text': 'AMC', 'indices': [252, 256]}, {'text': 'GME', 'indices': [257, 261]}, {'text': 'ShortSqueeze', 'indices': [263, 276]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [87, 92]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'CanadaNickel', 'indices': [152, 165]}, {'text': 'SudburyTwoPointO', 'indices': [167, 184]}, {'text': 'NetZeroNickel', 'indices': [185, 199]}, {'text': 'Nickel', 'indices': [201, 208]}, {'text': 'EV', 'indices': [225, 228]}, {'text': 'TSLA', 'indices': [230, 235]}, {'text': 'ESG', 'indices': [236, 240]}, {'text': 'Glencore', 'indices': [244, 253]}, {'text': 'BHP', 'indices': [254, 258]}, {'text': 'Vale', 'indices': [259, 264]}, {'text': 'Canada', 'indices': [265, 272]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [198, 203]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [36, 41]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [29, 34]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [25, 30]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [0, 5]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [30, 35]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [103, 108]}, {'text': 'wallstreetbets', 'indices': [112, 127]}, {'text': 'stocks', 'indices': [129, 136]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'AAPL', 'indices': [111, 116]}, {'text': 'TSLA', 'indices': [129, 134]}, {'text': 'NDX', 'indices': [140, 144]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [173, 178]}, {'text': 'FSDBetaCanada', 'indices': [179, 193]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [0, 5]}, {'text': 'Tesla', 'indices': [6, 12]}, {'text': 'Elon', 'indices': [13, 18]}, {'text': 'ElonMusk', 'indices': [19, 28]}, {'text': 'Bitcoin', 'indices': [42, 50]}, {'text': 'BTC', 'indices': [51, 55]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [9, 14]}, {'text': 'Tesla', 'indices': [15, 21]}, {'text': 'Elon', 'indices': [22, 27]}, {'text': 'ElonMusk', 'indices': [28, 37]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tesla', 'indices': [33, 39]}, {'text': 'builtTentTough', 'indices': [40, 55]}, {'text': 'tsla', 'indices': [56, 61]}, {'text': 'musked', 'indices': [72, 79]}, {'text': 'rookiemistake', 'indices': [195, 209]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [31, 36]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'ev', 'indices': [24, 27]}, {'text': 'tsla', 'indices': [28, 33]}, {'text': 'GreenNewDeal', 'indices': [34, 47]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'ev', 'indices': [84, 87]}, {'text': 'ElectricVehicles', 'indices': [88, 105]}, {'text': 'TSLA', 'indices': [106, 111]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [28, 33]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [218, 223]}, {'text': 'AMC', 'indices': [224, 228]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [111, 116]}, {'text': 'StockMarket', 'indices': [117, 129]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [79, 84]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'PLTR', 'indices': [29, 34]}, {'text': 'NIO', 'indices': [36, 40]}, {'text': 'TSLA', 'indices': [42, 47]}, {'text': 'RIOT', 'indices': [53, 58]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'HBAR', 'indices': [17, 22]}, {'text': 'TSLA', 'indices': [28, 33]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Tesla', 'indices': [26, 32]}, {'text': 'TSLA', 'indices': [34, 39]}, {'text': 'StockBuzzNow', 'indices': [217, 230]}, {'text': 'stockmarkettips', 'indices': [231, 247]}, {'text': 'usamarket', 'indices': [248, 258]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [51, 56]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Webull', 'indices': [85, 92]}, {'text': 'BTC', 'indices': [129, 133]}, {'text': 'MMAT', 'indices': [137, 142]}, {'text': 'TSLA', 'indices': [143, 148]}, {'text': 'YOMTVRaps', 'indices': [149, 159]}, {'text': 'HipHop', 'indices': [160, 167]}, {'text': 'Verzuz', 'indices': [168, 175]}, {'text': 'NFT', 'indices': [176, 180]}, {'text': 'Stocks', 'indices': [181, 188]}, {'text': 'Stockmarket', 'indices': [189, 201]}, {'text': 'NFTCommunity', 'indices': [202, 215]}, {'text': 'CarlosEMendez', 'indices': [216, 230]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'EVs', 'indices': [31, 35]}, {'text': 'TSLA', 'indices': [247, 252]}, {'text': 'F', 'indices': [253, 255]}, {'text': 'GM', 'indices': [256, 259]}, {'text': 'LCID', 'indices': [260, 265]}, {'text': 'RIVN', 'indices': [266, 271]}, {'text': 'NIO', 'indices': [272, 276]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [94, 99]}, {'text': 'Tesla', 'indices': [100, 106]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'options', 'indices': [78, 86]}, {'text': 'daytrading', 'indices': [87, 98]}, {'text': 'spy', 'indices': [99, 103]}, {'text': 'tsla', 'indices': [104, 109]}, {'text': 'amc', 'indices': [110, 114]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [75, 80]}, {'text': 'ElonMusk', 'indices': [81, 90]}, {'text': 'TSLA', 'indices': [91, 96]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [111, 116]}, {'text': 'ElonMusk', 'indices': [117, 126]}, {'text': 'TSLA', 'indices': [127, 132]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'Musk', 'indices': [84, 89]}, {'text': 'ElonMusk', 'indices': [90, 99]}, {'text': 'TSLA', 'indices': [100, 105]}]</t>
+    <t>Thoughts on $TSLA #TSLA! See zeyankhan1318's idea on TradingView below. https://t.co/nspRUd6puv</t>
+  </si>
+  <si>
+    <t>$TSLA Stock Split!!!
+ Here's what you need to know:
+https://t.co/amvs2gVhEN
+#tsla #teslastock #StockMarket #StockSplit #fintwit #FinTwitt</t>
+  </si>
+  <si>
+    <t>#TESLA #TSLA CHART REQUEST
+If trading leverage, consider taking some profit at current level. Likely to pullback to fill the parabola (lower range consolidation). If parabola remains intact, this could go to $1979 in a very short time. Risk manage at all times. All the best https://t.co/EtLgLsPj7z</t>
+  </si>
+  <si>
+    <t>Wednesday,  March 30, 2022
+Daily Market Correction : 
+🌙  Waning 5% in ♓️ 🍅 
+🐻‍❄️: 0654 - 0900 EST 
+🐃: 1002 - 1208 EST 
+🐻‍❄️: 1413 - 1619 EST
+🐃: 1722 - 1927 EST
+🐻‍❄️: 2121 - 2316 EST 
+$SPY #sp500 #Bitcoin $AAPL $NVDA $MSFT #TSLA #NASDAQ 
+(not financial advice)</t>
+  </si>
+  <si>
+    <t>@alex_avoigt But, but Gordon said the opening of Giga Berlin was a stock pump.  Berlin won’t deliver any cars anytime soon #TSLAQ #TSLA</t>
+  </si>
+  <si>
+    <t>#BTC #TSLA 
+Let's start to prepare NYO
+- $DXY : BreakDown Trend
+- $USOIL : Key-Horizontal level
+- $VIX : Dump. but support level
+- $GOLD : Range Low
+US stock 
+- $QQQ : HOLD around Range High
+- $AMD : No problem(imo)
+Crypto
+- $BTC : HOLD near RH https://t.co/bJaL3TI5YB</t>
+  </si>
+  <si>
+    <t>I want to buy #tsla</t>
+  </si>
+  <si>
+    <t>Is #TSLA a buy, hold or sell in its current value? #teslastock</t>
+  </si>
+  <si>
+    <t>@hikingskiing they direct listed, so institutional wallstreet does not like them.  i hold them long term, and software is high margin.  got #tsla back in 2010, and people were saying the same thing for many years.  same for #btc back in 2015.  hmm 🤔😂😂. HODL'ong &amp;amp; HODL'hard 👊👊</t>
+  </si>
+  <si>
+    <t>Have a look #Elonmusk #tsla #audi #volkswagen #porsche #mercedes #panasonic #varta #bmw #recycling #recycle #electricvehicle #batteries https://t.co/JifoClSnEj</t>
+  </si>
+  <si>
+    <t>@hikingskiing 99% sure for #tsla, #btc, #pltr.  95% for #eth, #ada</t>
+  </si>
+  <si>
+    <t>$TSLA seeing sustained chatter on wallstreetbets over the last few days_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #stocks https://t.co/9k2ryyKqd3</t>
+  </si>
+  <si>
+    <t>@stevenmarkryan Trust fund. Invest almost all 10M in #TSLA and growth stocks. Use excess to read books (a lot of books) and work at Tesla to make the planet better. #BuyTSLA</t>
+  </si>
+  <si>
+    <t>Thoughts on $TSLA #TSLA! See forextidings's idea on TradingView below. https://t.co/JwcxUipWYl</t>
+  </si>
+  <si>
+    <t>EWT: Tesla Has Brokendown The Corrective Structure - #TSLA chart on @TradingView https://t.co/8qYISdScPy</t>
+  </si>
+  <si>
+    <t>Bored to flip through the photo album, flip to the video I took before,  $TSLA Tesla’s Christmas mode is very fun, and there are many functions in the game box.#TSLA https://t.co/7W93sb4NvF</t>
+  </si>
+  <si>
+    <t>$TSLA will be at its lowest on 2022-03-30 best time to BUY #tsla #stockstobuy</t>
+  </si>
+  <si>
+    <t>$TSLA will be at its highest on 2023-03-29 best time to SELL #tsla #pips</t>
+  </si>
+  <si>
+    <t>Today Watchlist on market
+- #btc #US10Y #TSLA #AMD #nvda 
+- Market participant is scary on "10y2yt"
+- However, currently i dont much worry on it till next FOMC(May) #fomc #FederalReserve https://t.co/BhjPr515GD https://t.co/f7ZvyePrwY</t>
+  </si>
+  <si>
+    <t>Tesla..What Can You Say!! #tesla #tsla #stock #stockmarket #options #money #cars #tech #technology https://t.co/bYZi17GLz8</t>
+  </si>
+  <si>
+    <t>@topstonks The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@MissjanedivaCA The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@Zanttts The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>At the Tesla showroom in Singapore. Looking forward to seeing tsla exceed US$1,100 in the coming days, closer to giga texas’ opening.
+$tsla #TSLA https://t.co/FYdCYlejTW</t>
+  </si>
+  <si>
+    <t>MY WEBSITE HAS OFFICIALLY LAUNCHED https://t.co/TVtvJBQHLy #ETH #BTC #CRYPTO #cryptocurrency #cryptotrading #blockchain #TSLA</t>
+  </si>
+  <si>
+    <t>Tesla generates a lot of roadway video and map data everyday. SpaceX has the ability to cheaply launch satellites that can map the earth. 
+Will Tesla or SpaceX ever create map software or sell map data (i.e. Google/Apple Maps)?
+#TSLA @elonmusk #SpaceX #GoogleMaps #Maps #EV</t>
+  </si>
+  <si>
+    <t>@NapADayzzz The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@_Stock_Ideas The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@michaelnotts @RollsRoyce The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>@RealMiCentral The Big Lawsuit Against Elon Musk That The World is Talking About  #Musk #ElonMusk #TSLA  https://t.co/7Qr2O9qXf5</t>
+  </si>
+  <si>
+    <t>#dogecoin #TSLA #ElonMusk #shibainu Love this guy, he's so right, get a job, CRT Woke dumbasses . And quit whining about ur race. Lazy ass. https://t.co/6WniCxlbDL</t>
+  </si>
+  <si>
+    <t>Now that #tsla is basically at 1100, do you see it going first to 1200 or 1000?</t>
+  </si>
+  <si>
+    <t>Domain Name For Sale
+https://t.co/HSnQndMSr2
+.
+#Domains #domainnameforsale #domainsforsale #cryptocurrency #cryptotrading #Crypto #Cryptos #cryptogiveaway #CryptocurrencyNews #Bitcoin #cryptobank #cryptowallet #BTC #Ethereum #ETH #tezos #doge #TSLA #NFT #blockchain #Web3Coin #DAO https://t.co/rff3v24btU</t>
+  </si>
+  <si>
+    <t>https://t.co/gwyomrWBXo - Analyst ADMITS Legacy Auto Is DOOMED: Tesla Untouchable
+NEW
+$TSLA #Tesla #TSLA #TeslaStock #ElonMusk https://t.co/XwYi3bddGR</t>
+  </si>
+  <si>
+    <t>Domain Name For Sale
+https://t.co/oEUp6n6yi9
+.
+#Domains #domainnameforsale #domainsforsale #cryptocurrency #cryptotrading #Crypto #Cryptos #cryptogiveaway #CryptocurrencyNews #Bitcoin #cryptobank #cryptowallet #BTC #Ethereum #ETH #tezos #doge #TSLA #NFT #blockchain #Coinbase #DAO https://t.co/gTSTP2rSGi</t>
+  </si>
+  <si>
+    <t>If #TSLA @ $1000 p/share has a market cap of roughly 1 Trillion USD and there's a 10-for-1 split, 1 #Tesla stock would only need to go from $100 to $200 p/share to have a market cap of 2 Trillion USD.
+Not only is that possible in 2022, but highly probable. (IMO) https://t.co/9ZQuZ46BMT</t>
+  </si>
+  <si>
+    <t>$TSLA working its way into the top 10 most mentioned on wallstreetbets over the last 24 hours_x000D__x000D_Via https://t.co/gAloIO6Q7s_x000D__x000D_#tsla    #wallstreetbets  #investing https://t.co/TP92jolHqs</t>
+  </si>
+  <si>
+    <t>Why do other people still have flowers and bears in the car pick-up ceremony, but I don't? Is it because of the tense situation in Shanghai, the master driver sent it to my door, so I didn't have it?  $TSLA  #TSLA https://t.co/aHxmzsqmrt</t>
+  </si>
+  <si>
+    <t>#tesla #tsla Rudimentary drawing and rough percentages but see any patterns? 🚀🚀🚀 https://t.co/iMjGg1u2Kn</t>
+  </si>
+  <si>
+    <t>This was a solid entry today on #TSLA after almost 10 min period of consolidation, flag, and then break of the PML. https://t.co/3aMBszDT9F</t>
+  </si>
+  <si>
+    <t>@onepeloton @tune2tunde #Elonmusk .@elonmusk of #TSLA $TSLA should buyout this company #peloton #PTON $PTON throw a big wrench in #Apple $APPL Plans since .@Tesla  sell everything cars to even electricity.</t>
+  </si>
+  <si>
+    <t>When someone says https://t.co/rZ4CpCOsbr is real 
+@dogecoin  @elonmusk  @Tesla  
+27h nothing 
+____________________________________''________''________
+$TSLA #TSLA #doge $DOGE #ElonMusk #dogecoin #crypto #Exchange #WillSmith https://t.co/Pfg6DYsPnW</t>
+  </si>
+  <si>
+    <t>Sometimes the market just doesnt make sense right? 
+Like right now? It's been like 10+ days of straight green... its gotta retest on some point right? #SPY #TSLA #AMD #HOOD #SHOP #AMC</t>
+  </si>
+  <si>
+    <t>@elonmusk TRADING PLAN: TSLA 
+#Tesla #TSLA #stocks #StocksToTrade #StockMarket #ElonMusk #Elon 
+view more https://t.co/BqJMWNKnw8
+Please like &amp;amp; retweet this post. I love you 3000! https://t.co/eMCzwPUkZw</t>
+  </si>
+  <si>
+    <t>@elonmusk TRADING PLAN: TSLA 
+#Tesla #TSLA #stocks #StocksToTrade #StockMarket #ElonMusk #Elon 
+view more https://t.co/BqJMWNKnw8
+Please like &amp;amp; retweet this post. I love you 3000! https://t.co/w4hl7gmVmB</t>
+  </si>
+  <si>
+    <t>@elonmusk TRADING PLAN: TSLA 
+#Tesla #TSLA #stocks #StocksToTrade #StockMarket #ElonMusk #Elon 
+view more https://t.co/BqJMWNKnw8
+Please like &amp;amp; retweet this post. I love you 3000! https://t.co/iRNupNFVMO</t>
+  </si>
+  <si>
+    <t>TRADING PLAN: TSLA 
+#Tesla #TSLA #stocks #StocksToTrade #StockMarket #ElonMusk #Elon 
+view more https://t.co/BqJMWNKnw8
+Please like &amp;amp; retweet this post. I love you 3000! https://t.co/XTRWtApriA</t>
+  </si>
+  <si>
+    <t>Can somebody pls name another trader doing it like sickboytrades LLC #TSLA #SHOP #AMZN #SPY #ETH #BTC #NFT #OptionsTrading #daytrading https://t.co/hgsAaduAFv</t>
+  </si>
+  <si>
+    <t>NIU’s fastest and most powerful electric scooter yet arrives in Europe, headed to US soon - @elonmusk #TESLA #TSLA 
+https://t.co/eTLUGb7fF0 https://t.co/c8LXO71sgL</t>
+  </si>
+  <si>
+    <t>30-03-2022 10:33</t>
+  </si>
+  <si>
+    <t>30-03-2022 10:20</t>
+  </si>
+  <si>
+    <t>30-03-2022 10:15</t>
+  </si>
+  <si>
+    <t>30-03-2022 10:11</t>
+  </si>
+  <si>
+    <t>30-03-2022 09:34</t>
+  </si>
+  <si>
+    <t>30-03-2022 09:32</t>
+  </si>
+  <si>
+    <t>30-03-2022 09:28</t>
+  </si>
+  <si>
+    <t>30-03-2022 09:24</t>
+  </si>
+  <si>
+    <t>30-03-2022 09:11</t>
+  </si>
+  <si>
+    <t>30-03-2022 09:07</t>
+  </si>
+  <si>
+    <t>30-03-2022 08:55</t>
+  </si>
+  <si>
+    <t>30-03-2022 08:53</t>
+  </si>
+  <si>
+    <t>30-03-2022 08:23</t>
+  </si>
+  <si>
+    <t>30-03-2022 08:02</t>
+  </si>
+  <si>
+    <t>30-03-2022 07:58</t>
+  </si>
+  <si>
+    <t>30-03-2022 06:41</t>
+  </si>
+  <si>
+    <t>30-03-2022 06:28</t>
+  </si>
+  <si>
+    <t>30-03-2022 05:53</t>
+  </si>
+  <si>
+    <t>30-03-2022 05:36</t>
+  </si>
+  <si>
+    <t>30-03-2022 05:35</t>
+  </si>
+  <si>
+    <t>30-03-2022 05:34</t>
+  </si>
+  <si>
+    <t>30-03-2022 05:14</t>
+  </si>
+  <si>
+    <t>30-03-2022 05:05</t>
+  </si>
+  <si>
+    <t>30-03-2022 04:46</t>
+  </si>
+  <si>
+    <t>30-03-2022 04:38</t>
+  </si>
+  <si>
+    <t>30-03-2022 04:37</t>
+  </si>
+  <si>
+    <t>30-03-2022 04:36</t>
+  </si>
+  <si>
+    <t>30-03-2022 04:22</t>
+  </si>
+  <si>
+    <t>30-03-2022 03:46</t>
+  </si>
+  <si>
+    <t>30-03-2022 03:45</t>
+  </si>
+  <si>
+    <t>30-03-2022 03:42</t>
+  </si>
+  <si>
+    <t>30-03-2022 03:30</t>
+  </si>
+  <si>
+    <t>30-03-2022 03:26</t>
+  </si>
+  <si>
+    <t>30-03-2022 03:02</t>
+  </si>
+  <si>
+    <t>30-03-2022 02:30</t>
+  </si>
+  <si>
+    <t>30-03-2022 02:29</t>
+  </si>
+  <si>
+    <t>30-03-2022 01:08</t>
+  </si>
+  <si>
+    <t>30-03-2022 01:01</t>
+  </si>
+  <si>
+    <t>30-03-2022 00:56</t>
+  </si>
+  <si>
+    <t>30-03-2022 00:54</t>
+  </si>
+  <si>
+    <t>30-03-2022 00:38</t>
+  </si>
+  <si>
+    <t>30-03-2022 00:37</t>
+  </si>
+  <si>
+    <t>30-03-2022 00:36</t>
+  </si>
+  <si>
+    <t>30-03-2022 00:35</t>
+  </si>
+  <si>
+    <t>30-03-2022 00:31</t>
+  </si>
+  <si>
+    <t>29-09-2020 16:38</t>
+  </si>
+  <si>
+    <t>28-07-2009 02:25</t>
+  </si>
+  <si>
+    <t>23-04-2010 17:28</t>
+  </si>
+  <si>
+    <t>04-09-2018 16:36</t>
+  </si>
+  <si>
+    <t>24-05-2010 19:33</t>
+  </si>
+  <si>
+    <t>29-03-2022 02:15</t>
+  </si>
+  <si>
+    <t>04-12-2019 10:53</t>
+  </si>
+  <si>
+    <t>15-10-2011 23:44</t>
+  </si>
+  <si>
+    <t>03-04-2018 06:05</t>
+  </si>
+  <si>
+    <t>29-01-2021 14:40</t>
+  </si>
+  <si>
+    <t>08-01-2020 17:10</t>
+  </si>
+  <si>
+    <t>18-04-2018 05:40</t>
+  </si>
+  <si>
+    <t>22-09-2013 17:01</t>
+  </si>
+  <si>
+    <t>15-09-2021 08:17</t>
+  </si>
+  <si>
+    <t>04-07-2021 15:36</t>
+  </si>
+  <si>
+    <t>04-08-2017 02:58</t>
+  </si>
+  <si>
+    <t>06-12-2010 23:58</t>
+  </si>
+  <si>
+    <t>29-01-2022 01:28</t>
+  </si>
+  <si>
+    <t>29-02-2016 06:12</t>
+  </si>
+  <si>
+    <t>20-01-2014 02:58</t>
+  </si>
+  <si>
+    <t>28-02-2022 15:34</t>
+  </si>
+  <si>
+    <t>22-06-2020 00:03</t>
+  </si>
+  <si>
+    <t>08-02-2022 20:08</t>
+  </si>
+  <si>
+    <t>14-04-2009 23:28</t>
+  </si>
+  <si>
+    <t>02-03-2021 00:56</t>
+  </si>
+  <si>
+    <t>20-03-2022 02:57</t>
+  </si>
+  <si>
+    <t>03-11-2009 16:30</t>
+  </si>
+  <si>
+    <t>05-03-2021 06:00</t>
+  </si>
+  <si>
+    <t>01-11-2014 21:00</t>
+  </si>
+  <si>
+    <t>28-02-2022 16:27</t>
+  </si>
+  <si>
+    <t>29-05-2020 04:24</t>
+  </si>
+  <si>
+    <t>05-06-2012 02:22</t>
+  </si>
+  <si>
+    <t>17-02-2022 13:48</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [18, 23]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [79, 84]}, {'text': 'teslastock', 'indices': [85, 96]}, {'text': 'StockMarket', 'indices': [97, 109]}, {'text': 'StockSplit', 'indices': [110, 121]}, {'text': 'fintwit', 'indices': [122, 130]}, {'text': 'FinTwitt', 'indices': [131, 140]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TESLA', 'indices': [0, 6]}, {'text': 'TSLA', 'indices': [7, 12]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'sp500', 'indices': [190, 196]}, {'text': 'Bitcoin', 'indices': [197, 205]}, {'text': 'TSLA', 'indices': [224, 229]}, {'text': 'NASDAQ', 'indices': [230, 237]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLAQ', 'indices': [123, 129]}, {'text': 'TSLA', 'indices': [130, 135]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'BTC', 'indices': [0, 4]}, {'text': 'TSLA', 'indices': [5, 10]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [14, 19]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [3, 8]}, {'text': 'teslastock', 'indices': [51, 62]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [140, 145]}, {'text': 'btc', 'indices': [224, 228]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Elonmusk', 'indices': [12, 21]}, {'text': 'tsla', 'indices': [22, 27]}, {'text': 'audi', 'indices': [28, 33]}, {'text': 'volkswagen', 'indices': [34, 45]}, {'text': 'porsche', 'indices': [46, 54]}, {'text': 'mercedes', 'indices': [55, 64]}, {'text': 'panasonic', 'indices': [65, 75]}, {'text': 'varta', 'indices': [76, 82]}, {'text': 'bmw', 'indices': [83, 87]}, {'text': 'recycling', 'indices': [88, 98]}, {'text': 'recycle', 'indices': [99, 107]}, {'text': 'electricvehicle', 'indices': [108, 124]}, {'text': 'batteries', 'indices': [125, 135]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [27, 32]}, {'text': 'btc', 'indices': [34, 38]}, {'text': 'pltr', 'indices': [40, 45]}, {'text': 'eth', 'indices': [56, 60]}, {'text': 'ada', 'indices': [62, 66]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [102, 107]}, {'text': 'wallstreetbets', 'indices': [111, 126]}, {'text': 'stocks', 'indices': [128, 135]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [53, 58]}, {'text': 'BuyTSLA', 'indices': [165, 173]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [53, 58]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [160, 165]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [59, 64]}, {'text': 'stockstobuy', 'indices': [65, 77]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [61, 66]}, {'text': 'pips', 'indices': [67, 72]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'btc', 'indices': [28, 32]}, {'text': 'US10Y', 'indices': [33, 39]}, {'text': 'TSLA', 'indices': [40, 45]}, {'text': 'AMD', 'indices': [46, 50]}, {'text': 'nvda', 'indices': [51, 56]}, {'text': 'fomc', 'indices': [165, 170]}, {'text': 'FederalReserve', 'indices': [171, 186]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tesla', 'indices': [26, 32]}, {'text': 'tsla', 'indices': [33, 38]}, {'text': 'stock', 'indices': [39, 45]}, {'text': 'stockmarket', 'indices': [46, 58]}, {'text': 'options', 'indices': [59, 67]}, {'text': 'money', 'indices': [68, 74]}, {'text': 'cars', 'indices': [75, 80]}, {'text': 'tech', 'indices': [81, 86]}, {'text': 'technology', 'indices': [87, 98]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [78, 83]}, {'text': 'ElonMusk', 'indices': [84, 93]}, {'text': 'TSLA', 'indices': [94, 99]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [83, 88]}, {'text': 'ElonMusk', 'indices': [89, 98]}, {'text': 'TSLA', 'indices': [99, 104]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [76, 81]}, {'text': 'ElonMusk', 'indices': [82, 91]}, {'text': 'TSLA', 'indices': [92, 97]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [141, 146]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'ETH', 'indices': [59, 63]}, {'text': 'BTC', 'indices': [64, 68]}, {'text': 'CRYPTO', 'indices': [69, 76]}, {'text': 'cryptocurrency', 'indices': [77, 92]}, {'text': 'cryptotrading', 'indices': [93, 107]}, {'text': 'blockchain', 'indices': [108, 119]}, {'text': 'TSLA', 'indices': [120, 125]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [230, 235]}, {'text': 'SpaceX', 'indices': [246, 253]}, {'text': 'GoogleMaps', 'indices': [254, 265]}, {'text': 'Maps', 'indices': [266, 271]}, {'text': 'EV', 'indices': [272, 275]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [79, 84]}, {'text': 'ElonMusk', 'indices': [85, 94]}, {'text': 'TSLA', 'indices': [95, 100]}]</t>
   </si>
   <si>
     <t>[{'text': 'Musk', 'indices': [81, 86]}, {'text': 'ElonMusk', 'indices': [87, 96]}, {'text': 'TSLA', 'indices': [97, 102]}]</t>
   </si>
   <si>
-    <t>[{'text': 'tesla', 'indices': [26, 32]}, {'text': 'tsla', 'indices': [33, 38]}, {'text': 'stock', 'indices': [39, 45]}, {'text': 'stockmarket', 'indices': [46, 58]}, {'text': 'options', 'indices': [59, 67]}, {'text': 'money', 'indices': [68, 74]}, {'text': 'cars', 'indices': [75, 80]}, {'text': 'tech', 'indices': [81, 86]}, {'text': 'technology', 'indices': [87, 98]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'tsla', 'indices': [7, 12]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [18, 23]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [22, 27]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [11, 16]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'doge', 'indices': [25, 30]}, {'text': 'tsla', 'indices': [35, 40]}]</t>
-  </si>
-  <si>
-    <t>[{'text': 'TSLA', 'indices': [17, 22]}]</t>
+    <t>[{'text': 'Musk', 'indices': [93, 98]}, {'text': 'ElonMusk', 'indices': [99, 108]}, {'text': 'TSLA', 'indices': [109, 114]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Musk', 'indices': [82, 87]}, {'text': 'ElonMusk', 'indices': [88, 97]}, {'text': 'TSLA', 'indices': [98, 103]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'dogecoin', 'indices': [0, 9]}, {'text': 'TSLA', 'indices': [10, 15]}, {'text': 'ElonMusk', 'indices': [16, 25]}, {'text': 'shibainu', 'indices': [26, 35]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [9, 14]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Domains', 'indices': [47, 55]}, {'text': 'domainnameforsale', 'indices': [56, 74]}, {'text': 'domainsforsale', 'indices': [75, 90]}, {'text': 'cryptocurrency', 'indices': [91, 106]}, {'text': 'cryptotrading', 'indices': [107, 121]}, {'text': 'Crypto', 'indices': [122, 129]}, {'text': 'Cryptos', 'indices': [130, 138]}, {'text': 'cryptogiveaway', 'indices': [139, 154]}, {'text': 'CryptocurrencyNews', 'indices': [155, 174]}, {'text': 'Bitcoin', 'indices': [175, 183]}, {'text': 'cryptobank', 'indices': [184, 195]}, {'text': 'cryptowallet', 'indices': [196, 209]}, {'text': 'BTC', 'indices': [210, 214]}, {'text': 'Ethereum', 'indices': [215, 224]}, {'text': 'ETH', 'indices': [225, 229]}, {'text': 'tezos', 'indices': [230, 236]}, {'text': 'doge', 'indices': [237, 242]}, {'text': 'TSLA', 'indices': [243, 248]}, {'text': 'NFT', 'indices': [249, 253]}, {'text': 'blockchain', 'indices': [254, 265]}, {'text': 'Web3Coin', 'indices': [266, 275]}, {'text': 'DAO', 'indices': [276, 280]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [94, 100]}, {'text': 'TSLA', 'indices': [101, 106]}, {'text': 'TeslaStock', 'indices': [107, 118]}, {'text': 'ElonMusk', 'indices': [119, 128]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Domains', 'indices': [47, 55]}, {'text': 'domainnameforsale', 'indices': [56, 74]}, {'text': 'domainsforsale', 'indices': [75, 90]}, {'text': 'cryptocurrency', 'indices': [91, 106]}, {'text': 'cryptotrading', 'indices': [107, 121]}, {'text': 'Crypto', 'indices': [122, 129]}, {'text': 'Cryptos', 'indices': [130, 138]}, {'text': 'cryptogiveaway', 'indices': [139, 154]}, {'text': 'CryptocurrencyNews', 'indices': [155, 174]}, {'text': 'Bitcoin', 'indices': [175, 183]}, {'text': 'cryptobank', 'indices': [184, 195]}, {'text': 'cryptowallet', 'indices': [196, 209]}, {'text': 'BTC', 'indices': [210, 214]}, {'text': 'Ethereum', 'indices': [215, 224]}, {'text': 'ETH', 'indices': [225, 229]}, {'text': 'tezos', 'indices': [230, 236]}, {'text': 'doge', 'indices': [237, 242]}, {'text': 'TSLA', 'indices': [243, 248]}, {'text': 'NFT', 'indices': [249, 253]}, {'text': 'blockchain', 'indices': [254, 265]}, {'text': 'Coinbase', 'indices': [266, 275]}, {'text': 'DAO', 'indices': [276, 280]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [3, 8]}, {'text': 'Tesla', 'indices': [100, 106]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tsla', 'indices': [124, 129]}, {'text': 'wallstreetbets', 'indices': [133, 148]}, {'text': 'investing', 'indices': [150, 160]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [208, 213]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'tesla', 'indices': [0, 6]}, {'text': 'tsla', 'indices': [7, 12]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [32, 37]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Elonmusk', 'indices': [24, 33]}, {'text': 'TSLA', 'indices': [48, 53]}, {'text': 'peloton', 'indices': [87, 95]}, {'text': 'PTON', 'indices': [96, 101]}, {'text': 'Apple', 'indices': [130, 136]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [158, 163]}, {'text': 'doge', 'indices': [164, 169]}, {'text': 'ElonMusk', 'indices': [176, 185]}, {'text': 'dogecoin', 'indices': [186, 195]}, {'text': 'crypto', 'indices': [196, 203]}, {'text': 'Exchange', 'indices': [204, 213]}, {'text': 'WillSmith', 'indices': [214, 224]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'SPY', 'indices': [152, 156]}, {'text': 'TSLA', 'indices': [157, 162]}, {'text': 'AMD', 'indices': [163, 167]}, {'text': 'HOOD', 'indices': [168, 173]}, {'text': 'SHOP', 'indices': [174, 179]}, {'text': 'AMC', 'indices': [180, 184]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [31, 37]}, {'text': 'TSLA', 'indices': [38, 43]}, {'text': 'stocks', 'indices': [44, 51]}, {'text': 'StocksToTrade', 'indices': [52, 66]}, {'text': 'StockMarket', 'indices': [67, 79]}, {'text': 'ElonMusk', 'indices': [80, 89]}, {'text': 'Elon', 'indices': [90, 95]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'Tesla', 'indices': [21, 27]}, {'text': 'TSLA', 'indices': [28, 33]}, {'text': 'stocks', 'indices': [34, 41]}, {'text': 'StocksToTrade', 'indices': [42, 56]}, {'text': 'StockMarket', 'indices': [57, 69]}, {'text': 'ElonMusk', 'indices': [70, 79]}, {'text': 'Elon', 'indices': [80, 85]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TSLA', 'indices': [69, 74]}, {'text': 'SHOP', 'indices': [75, 80]}, {'text': 'AMZN', 'indices': [81, 86]}, {'text': 'SPY', 'indices': [87, 91]}, {'text': 'ETH', 'indices': [92, 96]}, {'text': 'BTC', 'indices': [97, 101]}, {'text': 'NFT', 'indices': [102, 106]}, {'text': 'OptionsTrading', 'indices': [107, 122]}, {'text': 'daytrading', 'indices': [123, 134]}]</t>
+  </si>
+  <si>
+    <t>[{'text': 'TESLA', 'indices': [102, 108]}, {'text': 'TSLA', 'indices': [109, 114]}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +631,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -531,16 +672,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -870,10 +1017,10 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -882,10 +1029,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -896,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>218561</v>
       </c>
       <c r="D3" t="s">
         <v>57</v>
@@ -908,10 +1055,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -922,22 +1069,22 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>31</v>
+        <v>1187</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -948,10 +1095,10 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>522</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -960,10 +1107,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="H5" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -974,10 +1121,10 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -986,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="H6" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1000,10 +1147,10 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1012,10 +1159,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="H7" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1026,10 +1173,10 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1038,10 +1185,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1052,10 +1199,10 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>331</v>
+        <v>156</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1064,10 +1211,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="H9" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1078,22 +1225,22 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>2309</v>
+        <v>646</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="H10" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1104,10 +1251,10 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>97</v>
+        <v>425</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1116,10 +1263,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="H11" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1130,10 +1277,10 @@
         <v>17</v>
       </c>
       <c r="C12">
-        <v>73</v>
+        <v>646</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1142,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="H12" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1156,10 +1303,10 @@
         <v>18</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3139</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1168,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1182,10 +1329,10 @@
         <v>19</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1194,10 +1341,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="H14" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1208,10 +1355,10 @@
         <v>20</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1220,10 +1367,10 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="H15" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1234,10 +1381,10 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>319</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1246,10 +1393,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1260,10 +1407,10 @@
         <v>22</v>
       </c>
       <c r="C17">
-        <v>3136</v>
+        <v>109</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1272,10 +1419,10 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1286,10 +1433,10 @@
         <v>23</v>
       </c>
       <c r="C18">
-        <v>40</v>
+        <v>1017</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1298,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="H18" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1312,10 +1459,10 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>823</v>
+        <v>1017</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1324,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="H19" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1338,10 +1485,10 @@
         <v>25</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1350,10 +1497,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="H20" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1364,10 +1511,10 @@
         <v>26</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>268</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1376,10 +1523,10 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="H21" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1390,10 +1537,10 @@
         <v>27</v>
       </c>
       <c r="C22">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1402,10 +1549,10 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1416,10 +1563,10 @@
         <v>28</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1428,10 +1575,10 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="H23" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1442,10 +1589,10 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1454,10 +1601,10 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="H24" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1468,10 +1615,10 @@
         <v>30</v>
       </c>
       <c r="C25">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1480,10 +1627,10 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="H25" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1494,10 +1641,10 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <v>17</v>
+        <v>296</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1506,10 +1653,10 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="H26" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1520,10 +1667,10 @@
         <v>32</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1532,10 +1679,10 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="H27" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1546,10 +1693,10 @@
         <v>33</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1558,10 +1705,10 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="H28" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1572,10 +1719,10 @@
         <v>34</v>
       </c>
       <c r="C29">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1584,10 +1731,10 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="H29" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1598,10 +1745,10 @@
         <v>35</v>
       </c>
       <c r="C30">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1610,10 +1757,10 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="H30" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1621,25 +1768,25 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C31">
-        <v>1147</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="H31" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1647,13 +1794,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32">
-        <v>949</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1662,10 +1809,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="H32" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1673,13 +1820,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33">
-        <v>226</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1688,10 +1835,10 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="H33" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1699,13 +1846,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34">
-        <v>797</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1714,10 +1861,10 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="H34" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1725,51 +1872,51 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35">
-        <v>629</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="H35" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>41</v>
+      <c r="B36" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C36">
-        <v>460</v>
+        <v>99579</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="H36" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1777,13 +1924,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1792,10 +1939,10 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="H37" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1803,13 +1950,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38">
         <v>43</v>
       </c>
-      <c r="C38">
-        <v>94</v>
-      </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1818,10 +1965,10 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="H38" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1829,13 +1976,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39">
-        <v>94</v>
+        <v>3139</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1844,10 +1991,10 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="H39" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1855,13 +2002,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1870,10 +2017,10 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="H40" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1881,13 +2028,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41">
-        <v>94</v>
+        <v>217</v>
       </c>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1896,10 +2043,10 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="H41" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1907,13 +2054,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1922,10 +2069,10 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="H42" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1933,13 +2080,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43">
-        <v>269</v>
+        <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1948,10 +2095,10 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="H43" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1959,13 +2106,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1974,10 +2121,10 @@
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="H44" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1985,13 +2132,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45">
-        <v>53</v>
+        <v>775</v>
       </c>
       <c r="D45" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -2000,10 +2147,10 @@
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="H45" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2011,13 +2158,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46">
-        <v>1341</v>
+        <v>832</v>
       </c>
       <c r="D46" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2026,10 +2173,10 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H46" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2037,13 +2184,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47">
-        <v>10</v>
+        <v>832</v>
       </c>
       <c r="D47" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -2052,10 +2199,10 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="H47" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2063,13 +2210,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48">
-        <v>3257</v>
+        <v>832</v>
       </c>
       <c r="D48" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2078,10 +2225,10 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="H48" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2089,13 +2236,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49">
-        <v>781</v>
+        <v>832</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2104,10 +2251,10 @@
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="H49" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2115,13 +2262,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50">
-        <v>118</v>
+        <v>296</v>
       </c>
       <c r="D50" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2130,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="H50" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2141,13 +2288,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51">
-        <v>266</v>
+        <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2156,13 +2303,16 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="H51" t="s">
-        <v>100</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B36" r:id="rId1" location="Tesla%20#TSLA%20#TeslaStock%20#ElonMusk%20https://t.co/XwYi3bddGR"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>